<commit_message>
integrated wiadImageID and ownerImageID as well as bounding latitudes and longitudes in the metadata. Also dealt with some minor issues.
</commit_message>
<xml_diff>
--- a/inst/demos/WIAD-metadata-template-2020-09-14.xlsx
+++ b/inst/demos/WIAD-metadata-template-2020-09-14.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t xml:space="preserve">Your name</t>
   </si>
@@ -50,6 +50,18 @@
   </si>
   <si>
     <t xml:space="preserve">Site Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Lat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Lat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Lon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Lon</t>
   </si>
   <si>
     <t xml:space="preserve">Site ID</t>
@@ -109,7 +121,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
@@ -203,38 +215,36 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="21.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="8" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -292,63 +302,85 @@
       <c r="R1" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>44047</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>3600</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <f aca="false">FALSE()</f>
+        <v>3200</v>
+      </c>
+      <c r="H2" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I2" s="3" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="I2" s="3" t="b">
         <v>1</v>
       </c>
       <c r="J2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>42.513333</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>42.513333</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>-72.2183333</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>-72.2183333</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>